<commit_message>
- insert directory testscript
</commit_message>
<xml_diff>
--- a/excel/TC01_SearchIDCardType.xlsx
+++ b/excel/TC01_SearchIDCardType.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\IT496 Project IN Information Technology (AJ.SAYAN)\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\IT496 Project IN Information Technology (AJ.SAYAN)\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A1A1D1-FD8A-4B7C-A7B4-66FC8BE3BC94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373AB583-B828-4AA3-B9CA-4FE6D8EA9F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{02CACE61-8A48-4707-AED0-8E7ADDC3B807}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{02CACE61-8A48-4707-AED0-8E7ADDC3B807}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>Result</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>“กรุณากรอกข้อมูลให้ถูกต้อง”</t>
-  </si>
-  <si>
     <t>Progress Dialog</t>
   </si>
   <si>
@@ -182,6 +179,15 @@
   </si>
   <si>
     <t>9578958645780</t>
+  </si>
+  <si>
+    <t>"เลขรหัสประจำตัว 13 หลักไม่ถูกต้อง"</t>
+  </si>
+  <si>
+    <t>"กรุณากรอกข้อมูล?"</t>
+  </si>
+  <si>
+    <t>"ไม่พบประเภทบัตรบุคคลไร้รัฐไร้สัญชาติ"</t>
   </si>
 </sst>
 </file>
@@ -747,27 +753,27 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="1"/>
-    <col min="3" max="3" width="23.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.25" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="15.625" style="1"/>
+    <col min="1" max="1" width="10.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" style="1"/>
+    <col min="3" max="3" width="23.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.19921875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="15.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24">
+    <row r="1" spans="1:6" ht="24.6">
       <c r="A1" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>14</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>4</v>
@@ -776,18 +782,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="24">
+    <row r="2" spans="1:6" ht="24.6">
       <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>6</v>
@@ -803,46 +809,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B61F3A9-364F-42E3-A769-E210CEB40008}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="27" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="27" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
-    <col min="2" max="2" width="19.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="14.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.8984375" style="1"/>
+    <col min="2" max="2" width="19.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.8984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.09765625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="14.19921875" style="1" customWidth="1"/>
     <col min="6" max="6" width="55.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="1"/>
+    <col min="7" max="7" width="22.8984375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24">
+    <row r="1" spans="1:10" ht="24.6">
       <c r="A1" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>21</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>22</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>0</v>
@@ -851,119 +857,119 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24">
+    <row r="2" spans="1:10" ht="24.6">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="24">
+    <row r="3" spans="1:10" ht="24.6">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>39</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="24">
+    <row r="4" spans="1:10" ht="24.6">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="F4" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="24">
+    <row r="5" spans="1:10" ht="24.6">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F5" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="24">
+    <row r="6" spans="1:10" ht="24.6">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -981,31 +987,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D88CB84-7895-4465-A78B-6A22CB5104B1}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="24"/>
+  <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="24.6"/>
   <cols>
-    <col min="1" max="1" width="14.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="74.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.625" style="1"/>
-    <col min="7" max="7" width="23.75" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="15.625" style="1"/>
+    <col min="1" max="1" width="14.09765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="69.09765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.59765625" style="1"/>
+    <col min="7" max="7" width="23.69921875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="15.59765625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -1017,105 +1023,105 @@
         <v>0</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="23.45" customHeight="1">
+    <row r="2" spans="1:8" ht="23.4" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="23.45" customHeight="1">
+    <row r="3" spans="1:8" ht="23.4" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="23.45" customHeight="1">
+    <row r="4" spans="1:8" ht="23.4" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="23.45" customHeight="1">
+    <row r="5" spans="1:8" ht="23.4" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="23.45" customHeight="1">
+    <row r="6" spans="1:8" ht="23.4" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="2"/>

</xml_diff>

<commit_message>
- edit keyword/driver/StartUp/Keyword - add MyMobileActions
</commit_message>
<xml_diff>
--- a/excel/TC01_SearchIDCardType.xlsx
+++ b/excel/TC01_SearchIDCardType.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\IT496 Project IN Information Technology (AJ.SAYAN)\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DB276E-26CE-46DB-9C1C-B65350D5DAF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1CBAF7-1A7C-4681-B348-48B26A49F212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{02CACE61-8A48-4707-AED0-8E7ADDC3B807}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{02CACE61-8A48-4707-AED0-8E7ADDC3B807}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="4" r:id="rId1"/>
@@ -22,17 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Result</t>
   </si>
@@ -109,9 +104,6 @@
     <t>vAPK</t>
   </si>
   <si>
-    <t>Enter PersonID in PersonID Field</t>
-  </si>
-  <si>
     <t>edit_input</t>
   </si>
   <si>
@@ -169,25 +161,31 @@
     <t>TDID05</t>
   </si>
   <si>
-    <t>หน้าจอจะแสดงข้อมูลผู้ใช้</t>
-  </si>
-  <si>
     <t>9578958645780</t>
   </si>
   <si>
-    <t>"เลขรหัสประจำตัว 13 หลักไม่ถูกต้อง"</t>
-  </si>
-  <si>
-    <t>"กรุณากรอกข้อมูล?"</t>
-  </si>
-  <si>
-    <t>"ไม่พบประเภทบัตรบุคคลไร้รัฐไร้สัญชาติ"</t>
-  </si>
-  <si>
-    <t>open_app</t>
-  </si>
-  <si>
-    <t>close_app</t>
+    <t>Enter PersonID in Field</t>
+  </si>
+  <si>
+    <t>apk_open</t>
+  </si>
+  <si>
+    <t>apk_close</t>
+  </si>
+  <si>
+    <t>เลขรหัสประจำตัว 13 หลักไม่ถูกต้อง</t>
+  </si>
+  <si>
+    <t>ไม่พบประเภทบัตรบุคคลไร้รัฐไร้สัญชาติ</t>
+  </si>
+  <si>
+    <t>กรุณากรอกข้อมูล</t>
+  </si>
+  <si>
+    <t>หน้าจอแสดงข้อมูลผู้ใช้งาน</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -351,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -403,6 +401,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -750,7 +751,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="30" customHeight="1"/>
@@ -796,7 +797,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="F2" s="13"/>
     </row>
@@ -809,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B61F3A9-364F-42E3-A769-E210CEB40008}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="27" customHeight="1"/>
@@ -827,7 +828,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="24.6">
       <c r="A1" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>16</v>
@@ -839,7 +840,7 @@
         <v>18</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>19</v>
@@ -871,7 +872,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>24</v>
@@ -892,13 +893,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>35</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>36</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -916,16 +917,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F4" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -942,13 +943,13 @@
         <v>4</v>
       </c>
       <c r="D5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F5" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -966,10 +967,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -987,31 +988,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D88CB84-7895-4465-A78B-6A22CB5104B1}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="24.6"/>
+  <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="27" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.09765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.19921875" style="1" customWidth="1"/>
     <col min="3" max="3" width="69.09765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.19921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.8984375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.59765625" style="1"/>
     <col min="7" max="7" width="23.69921875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="15.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="27" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -1029,99 +1030,99 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="23.4" customHeight="1">
+    <row r="2" spans="1:8" ht="27" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>45</v>
+      <c r="E2" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="23.4" customHeight="1">
+    <row r="3" spans="1:8" ht="27" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>49</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="23.4" customHeight="1">
+    <row r="4" spans="1:8" ht="27" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>47</v>
+      <c r="E4" s="15" t="s">
+        <v>48</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="23.4" customHeight="1">
+    <row r="5" spans="1:8" ht="27" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>47</v>
+      <c r="E5" s="15" t="s">
+        <v>48</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="23.4" customHeight="1">
+    <row r="6" spans="1:8" ht="27" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="2" t="s">
-        <v>48</v>
+      <c r="E6" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="2"/>

</xml_diff>